<commit_message>
Modify the name of the filter title.lua to article-metadata.lua
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_virtual\Otros ordenadores\Mi portátil\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E6C70-4D3C-434B-A19A-8D8556F441C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="8610" activeTab="1"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19563" windowHeight="10162" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="type" sheetId="2" r:id="rId1"/>
@@ -36,9 +37,6 @@
     <t>md</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>unhighlight</t>
   </si>
   <si>
@@ -208,12 +206,15 @@
   </si>
   <si>
     <t>custom</t>
+  </si>
+  <si>
+    <t>article-metadata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,48 +543,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -595,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
@@ -603,126 +604,126 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -732,44 +733,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -786,7 +787,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -803,7 +804,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -811,7 +812,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -825,7 +826,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -839,7 +840,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -853,7 +854,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -865,16 +866,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -885,24 +886,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -910,7 +911,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -918,7 +919,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -926,7 +927,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -934,7 +935,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -942,7 +943,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -950,7 +951,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -958,7 +959,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -966,7 +967,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -974,7 +975,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -991,7 +992,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1005,7 +1006,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1023,100 +1024,100 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1127,80 +1128,80 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,44 +1214,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1264,7 +1265,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1281,7 +1282,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1289,7 +1290,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1300,7 +1301,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1314,7 +1315,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1328,7 +1329,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1336,21 +1337,21 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add doi-builder to pandoc_options
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8030849F-3A3A-48A1-8D85-F1302D8D1125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E30AFA-54EF-4D12-AE88-E9A28BCE44DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19563" windowHeight="10162" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="type" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="type (2)" sheetId="4" r:id="rId4"/>
     <sheet name="opts (2)" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>filter</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>translate-elements</t>
+  </si>
+  <si>
+    <t>doi-builder</t>
+  </si>
+  <si>
+    <t>crossref</t>
+  </si>
+  <si>
+    <t>--ascii=true</t>
   </si>
 </sst>
 </file>
@@ -258,12 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,19 +554,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.25" customWidth="1"/>
+    <col min="2" max="5" width="12.25" customWidth="1"/>
+    <col min="7" max="8" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -572,14 +583,17 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -595,14 +609,15 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -618,14 +633,15 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -641,14 +657,15 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -664,14 +681,15 @@
       <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -679,7 +697,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -687,7 +705,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -701,7 +719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -714,8 +732,11 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -734,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -745,7 +766,7 @@
     <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -761,14 +782,17 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -784,8 +808,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -798,19 +825,23 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -820,11 +851,14 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -834,11 +868,14 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -848,17 +885,34 @@
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -867,10 +921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -878,7 +932,7 @@
     <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,14 +948,17 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -909,114 +966,122 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Split 'author-to-canonical' and 'country-codes'
* Se agrega 'country-codes' a pandoc_options.
* Se simplifica código de author-to.canonical.
* Se modifica meta.institute para que no sea una copia de meta.affiliation (reduciendo los campos de meta.institute a 'index' y 'name').
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E51EF7B-9993-4211-BF28-1C2E04BD2A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCA930B-0073-474F-A9C5-112D8E7F20DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>filter</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>language-elements</t>
+  </si>
+  <si>
+    <t>country-codes</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1012,16 +1015,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" s="9">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>5</v>
       </c>
       <c r="B9" s="9">
         <v>8</v>
@@ -1029,17 +1032,17 @@
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="A10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
         <v>9</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B11" s="10">
         <v>10</v>
@@ -1048,7 +1051,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B12" s="10">
         <v>11</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="10">
         <v>12</v>
@@ -1066,48 +1069,57 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B14" s="10">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregar traducción para paratexto (credit & ack) y date
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079D0D7-DE15-43BE-B705-9469478E3266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E1CF15-8F12-4B93-8764-F11650588FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>metadata-format-in-text</t>
   </si>
   <si>
-    <t>latex-prepare</t>
-  </si>
-  <si>
     <t>xml</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>zotero-SuppressAuthor</t>
+  </si>
+  <si>
+    <t>babel-lang</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -588,21 +588,21 @@
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -615,7 +615,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>1</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -632,123 +632,123 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +772,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -787,18 +787,18 @@
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -925,10 +925,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -953,18 +953,18 @@
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7">
         <v>4</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7">
         <v>7</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="10">
         <v>11</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="10">
         <v>12</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1129,9 +1129,6 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
guri_clean_temp & AST/biblio files
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E1CF15-8F12-4B93-8764-F11650588FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4C69D2-3E53-4FC7-8ECB-84E7B488B5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="type" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>filter</t>
   </si>
@@ -89,9 +89,6 @@
     <t>latex</t>
   </si>
   <si>
-    <t>json</t>
-  </si>
-  <si>
     <t>option</t>
   </si>
   <si>
@@ -125,12 +122,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>VER: csljson/biblatex</t>
-  </si>
-  <si>
-    <t>_AST.json</t>
-  </si>
-  <si>
     <t>file_ext_input</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t>docx</t>
   </si>
   <si>
-    <t>json/bib</t>
-  </si>
-  <si>
     <t>biblio</t>
   </si>
   <si>
@@ -192,6 +180,9 @@
   </si>
   <si>
     <t>babel-lang</t>
+  </si>
+  <si>
+    <t>native</t>
   </si>
 </sst>
 </file>
@@ -265,13 +256,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -558,22 +548,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.25" customWidth="1"/>
-    <col min="7" max="8" width="12.25" customWidth="1"/>
+    <col min="2" max="6" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -587,22 +576,19 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -613,17 +599,14 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -637,17 +620,14 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -661,17 +641,14 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -685,36 +662,33 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -723,32 +697,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -770,9 +744,9 @@
     <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -786,19 +760,16 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -812,13 +783,13 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -829,25 +800,25 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -855,16 +826,16 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -872,16 +843,16 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
         <v>4</v>
       </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -889,34 +860,31 @@
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
         <v>5</v>
       </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -925,10 +893,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -936,14 +904,14 @@
     <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -952,143 +920,140 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="7">
+        <v>47</v>
+      </c>
+      <c r="B8" s="6">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>8</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="10">
+        <v>49</v>
+      </c>
+      <c r="B12" s="9">
         <v>11</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="10">
+        <v>48</v>
+      </c>
+      <c r="B13" s="9">
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>13</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>14</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1101,11 +1066,8 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1115,19 +1077,16 @@
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pandoc_options to include crossref
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4C69D2-3E53-4FC7-8ECB-84E7B488B5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA40C305-A1F3-4EF7-B6DD-1936B38F0D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>filter</t>
   </si>
@@ -71,9 +71,6 @@
     <t>metadata-format-in-text</t>
   </si>
   <si>
-    <t>xml</t>
-  </si>
-  <si>
     <t>AST</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>file_ext_output</t>
   </si>
   <si>
-    <t>docx</t>
-  </si>
-  <si>
     <t>biblio</t>
   </si>
   <si>
@@ -183,6 +177,42 @@
   </si>
   <si>
     <t>native</t>
+  </si>
+  <si>
+    <t>crossref-autaff</t>
+  </si>
+  <si>
+    <t>crossref-citation</t>
+  </si>
+  <si>
+    <t>scielo</t>
+  </si>
+  <si>
+    <t>crossref-resource-builder</t>
+  </si>
+  <si>
+    <t>crossref-register-prepare</t>
+  </si>
+  <si>
+    <t>%a.md</t>
+  </si>
+  <si>
+    <t>%a.html</t>
+  </si>
+  <si>
+    <t>%a.xml</t>
+  </si>
+  <si>
+    <t>%a.tex</t>
+  </si>
+  <si>
+    <t>%a_crossref.xml</t>
+  </si>
+  <si>
+    <t>%a.docx</t>
+  </si>
+  <si>
+    <t>%a_AST.native</t>
   </si>
 </sst>
 </file>
@@ -206,18 +236,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -256,18 +280,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,21 +574,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="12.25" customWidth="1"/>
+    <col min="2" max="8" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -577,153 +603,175 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B8" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -733,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -744,9 +792,9 @@
     <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -761,15 +809,18 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -783,13 +834,14 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -801,24 +853,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="12"/>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -827,15 +880,16 @@
         <v>3</v>
       </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -844,15 +898,16 @@
         <v>4</v>
       </c>
       <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="G6" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -861,30 +916,33 @@
         <v>5</v>
       </c>
       <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="G7" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
+      <c r="G9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -893,25 +951,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -920,140 +979,157 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="3"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="9">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="9">
+        <v>46</v>
+      </c>
+      <c r="B13" s="7">
         <v>12</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="3"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>13</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>14</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1066,8 +1142,9 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1077,17 +1154,52 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="10">
+        <v>4</v>
+      </c>
+      <c r="G22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add codemeta.json & Project Status badge
</commit_message>
<xml_diff>
--- a/data-raw/pandoc_options.xlsx
+++ b/data-raw/pandoc_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\_investigacion\99_Otros-proyectos\guri\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B3E52-CB39-4537-AE29-26725F4B7CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DA8478-BC7F-493B-8BAF-69F6E7B69EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>filter</t>
   </si>
@@ -170,9 +170,6 @@
     <t>zotero-translate</t>
   </si>
   <si>
-    <t>zotero-SuppressAuthor</t>
-  </si>
-  <si>
     <t>babel-lang</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>book-info</t>
+  </si>
+  <si>
+    <t>%a_scielo.xml</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
@@ -608,7 +610,7 @@
         <v>41</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
@@ -619,25 +621,25 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -645,23 +647,25 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="12"/>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,7 +687,9 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
@@ -707,9 +713,11 @@
       <c r="F5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,7 +727,6 @@
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -728,7 +735,6 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -743,7 +749,6 @@
       <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -761,7 +766,9 @@
       <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -773,7 +780,6 @@
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -786,7 +792,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="D5" sqref="D5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -814,7 +820,7 @@
         <v>41</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
@@ -839,7 +845,9 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -857,7 +865,9 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3">
+        <v>2</v>
+      </c>
       <c r="H3">
         <v>1</v>
       </c>
@@ -869,7 +879,6 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -884,7 +893,9 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5">
+        <v>3</v>
+      </c>
       <c r="H5">
         <v>2</v>
       </c>
@@ -902,7 +913,9 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6">
+        <v>4</v>
+      </c>
       <c r="H6">
         <v>3</v>
       </c>
@@ -920,7 +933,9 @@
       <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7">
+        <v>5</v>
+      </c>
       <c r="H7">
         <v>4</v>
       </c>
@@ -935,7 +950,9 @@
       <c r="F8">
         <v>6</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -944,7 +961,6 @@
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="G9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,10 +969,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -985,7 +1001,7 @@
         <v>41</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>14</v>
@@ -1093,7 +1109,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="7">
         <v>11</v>
@@ -1103,7 +1119,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B13" s="7">
         <v>12</v>
@@ -1113,7 +1129,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="7">
         <v>13</v>
@@ -1123,95 +1139,87 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="G15" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18">
+        <v>47</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18">
         <v>3</v>
       </c>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
       </c>
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F21" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F22" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="10">
-        <v>4</v>
-      </c>
-      <c r="G23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>